<commit_message>
he realizado otro cambio
</commit_message>
<xml_diff>
--- a/aula4.xlsx
+++ b/aula4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temporal\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB107F1-1ACC-4877-A828-1FED552D1973}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E8A7E5-77F2-4AAB-B75A-DDC6522F0992}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="2" xr2:uid="{703322BC-5837-41AF-AE09-2AA4EA37FA63}"/>
   </bookViews>
@@ -2027,7 +2027,7 @@
   <dimension ref="C4:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2162,6 +2162,11 @@
     </row>
     <row r="11" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N14">

</xml_diff>